<commit_message>
committing prior to refactor of eda_plotting
</commit_message>
<xml_diff>
--- a/reports/revenue_weather_models_mlr_results.xlsx
+++ b/reports/revenue_weather_models_mlr_results.xlsx
@@ -9,16 +9,16 @@
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="avg_base_passenger_fare_resid ~" sheetId="2" r:id="rId2"/>
-    <sheet name="fare_per_mile_resid ~ rain_flag" sheetId="3" r:id="rId3"/>
-    <sheet name="margin_per_mile_resid ~ rain_fl" sheetId="4" r:id="rId4"/>
-    <sheet name="driverpay_per_mile_resid ~ rain" sheetId="5" r:id="rId5"/>
+    <sheet name="fare_per_mile_resid ~ avg_trip_" sheetId="3" r:id="rId3"/>
+    <sheet name="margin_per_mile_resid ~ avg_tri" sheetId="4" r:id="rId4"/>
+    <sheet name="driverpay_per_mile_resid ~ avg_" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="67">
   <si>
     <t>model_label</t>
   </si>
@@ -131,16 +131,31 @@
     <t>p_8</t>
   </si>
   <si>
-    <t>avg_base_passenger_fare_resid ~ rain_flag_lag0 + rain_flag_lag1</t>
-  </si>
-  <si>
-    <t>fare_per_mile_resid ~ rain_flag_lag0 + rain_flag_lag1</t>
-  </si>
-  <si>
-    <t>margin_per_mile_resid ~ rain_flag_lag0 + rain_flag_lag1</t>
-  </si>
-  <si>
-    <t>driverpay_per_mile_resid ~ rain_flag_lag0 + rain_flag_lag1</t>
+    <t>avg_base_passenger_fare_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare</t>
+  </si>
+  <si>
+    <t>fare_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare</t>
+  </si>
+  <si>
+    <t>margin_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare</t>
+  </si>
+  <si>
+    <t>avg_base_passenger_fare_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f</t>
+  </si>
+  <si>
+    <t>fare_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f</t>
+  </si>
+  <si>
+    <t>margin_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f</t>
+  </si>
+  <si>
+    <t>driverpay_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + driver_pay_pct_of_base_fare + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f</t>
+  </si>
+  <si>
+    <t>driverpay_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f</t>
+  </si>
+  <si>
+    <t>driverpay_per_mile_resid ~ avg_trip_miles + avg_trip_time_min + demand_resid + rain_flag_lag0 + heavy_rain_flag_lag0 + precip_1h_mm_total + wind_chill_f + driver_pay_pct_of_base_fare</t>
   </si>
   <si>
     <t>avg_base_passenger_fare_resid</t>
@@ -685,7 +700,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>0.5700277732421278</v>
@@ -700,10 +715,10 @@
         <v>2.413322963547684</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -712,10 +727,10 @@
         <v>-0.02707074504635856</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M2">
         <v>0.001044524311421225</v>
@@ -724,10 +739,10 @@
         <v>0.00920773381084258</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q2">
         <v>3.360981872780581E-100</v>
@@ -736,10 +751,10 @@
         <v>-15.10301827160371</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U2">
         <v>3.151040359724815E-44</v>
@@ -750,7 +765,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>0.3128271537038596</v>
@@ -765,10 +780,10 @@
         <v>-0.07054833235873853</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I3">
         <v>2.763972244430455E-162</v>
@@ -777,10 +792,10 @@
         <v>0.005847306574090874</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M3">
         <v>9.611821080164007E-21</v>
@@ -789,10 +804,10 @@
         <v>0.0005977826922454803</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q3">
         <v>3.231492481229298E-75</v>
@@ -801,10 +816,10 @@
         <v>-2.653500839497895</v>
       </c>
       <c r="S3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U3">
         <v>2.60113504560505E-215</v>
@@ -815,7 +830,7 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>0.5849486296720854</v>
@@ -830,10 +845,10 @@
         <v>-0.01361209660142907</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I4">
         <v>6.775114198601769E-27</v>
@@ -842,10 +857,10 @@
         <v>-0.006825383736215593</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M4">
         <v>1.722307101570335E-101</v>
@@ -854,10 +869,10 @@
         <v>0.0002349890012747522</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q4">
         <v>1.963298150089567E-47</v>
@@ -866,10 +881,10 @@
         <v>-3.442523621864735</v>
       </c>
       <c r="S4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -877,10 +892,10 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>0.5976090290864393</v>
@@ -895,10 +910,10 @@
         <v>2.567281204183598</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I5">
         <v>1.095614597131088E-308</v>
@@ -907,10 +922,10 @@
         <v>-0.1813356063920056</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M5">
         <v>6.058288625263461E-23</v>
@@ -919,10 +934,10 @@
         <v>0.01017486372989804</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q5">
         <v>4.558608831814345E-26</v>
@@ -931,10 +946,10 @@
         <v>-13.30246450329206</v>
       </c>
       <c r="S5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U5">
         <v>5.166765734714298E-14</v>
@@ -943,10 +958,10 @@
         <v>1.924636689693848</v>
       </c>
       <c r="W5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Y5">
         <v>0.0008057928669036327</v>
@@ -955,7 +970,7 @@
         <v>-0.930796885552617</v>
       </c>
       <c r="AA5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AC5">
         <v>0.7955216691602308</v>
@@ -964,7 +979,7 @@
         <v>0.2974253892846115</v>
       </c>
       <c r="AE5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AG5">
         <v>0.4316024910641845</v>
@@ -973,7 +988,7 @@
         <v>-0.005395067678689072</v>
       </c>
       <c r="AI5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AK5">
         <v>0.6131247522578159</v>
@@ -981,10 +996,10 @@
     </row>
     <row r="6" spans="1:37">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>0.3210077657739525</v>
@@ -999,10 +1014,10 @@
         <v>-0.05361111238026152</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I6">
         <v>1.45483106371878E-34</v>
@@ -1011,10 +1026,10 @@
         <v>-0.007370480527641051</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M6">
         <v>1.662650768983388E-07</v>
@@ -1023,10 +1038,10 @@
         <v>0.0005697668442642861</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q6">
         <v>1.346998547516964E-14</v>
@@ -1035,10 +1050,10 @@
         <v>-2.616101958511456</v>
       </c>
       <c r="S6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U6">
         <v>1.826850878707894E-75</v>
@@ -1047,10 +1062,10 @@
         <v>0.152402554115701</v>
       </c>
       <c r="W6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Y6">
         <v>0.0006040271222392212</v>
@@ -1059,10 +1074,10 @@
         <v>-0.6078726742980095</v>
       </c>
       <c r="AA6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AB6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AC6">
         <v>0.02878762954655125</v>
@@ -1071,10 +1086,10 @@
         <v>0.07723276611382776</v>
       </c>
       <c r="AE6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AF6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AG6">
         <v>0.008348060303740305</v>
@@ -1083,7 +1098,7 @@
         <v>0.001293971855322156</v>
       </c>
       <c r="AI6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AK6">
         <v>0.1170666019777796</v>
@@ -1091,10 +1106,10 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>0.6049553546031476</v>
@@ -1109,10 +1124,10 @@
         <v>-0.006071572838217493</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I7">
         <v>0.006359329001445982</v>
@@ -1121,10 +1136,10 @@
         <v>-0.01330893776524718</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M7">
         <v>1.776605897839431E-68</v>
@@ -1133,10 +1148,10 @@
         <v>0.0002590361458050593</v>
       </c>
       <c r="O7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q7">
         <v>1.428234154658986E-11</v>
@@ -1145,10 +1160,10 @@
         <v>-3.373879094620659</v>
       </c>
       <c r="S7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U7">
         <v>1.976262583364986E-322</v>
@@ -1157,10 +1172,10 @@
         <v>0.09494968269543617</v>
       </c>
       <c r="W7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Y7">
         <v>3.928542927132261E-05</v>
@@ -1169,10 +1184,10 @@
         <v>-0.3518117003335053</v>
       </c>
       <c r="AA7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AB7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AC7">
         <v>0.0148424474521775</v>
@@ -1181,10 +1196,10 @@
         <v>0.0330772862006062</v>
       </c>
       <c r="AE7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AF7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AG7">
         <v>0.02956140185377016</v>
@@ -1193,10 +1208,10 @@
         <v>0.001994053441914628</v>
       </c>
       <c r="AI7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AJ7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="AK7">
         <v>3.517625792160124E-06</v>
@@ -1204,10 +1219,10 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>0.3210077657739525</v>
@@ -1222,10 +1237,10 @@
         <v>-0.05361111238026152</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I8">
         <v>1.45483106371878E-34</v>
@@ -1234,10 +1249,10 @@
         <v>-0.007370480527641051</v>
       </c>
       <c r="K8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M8">
         <v>1.662650768983388E-07</v>
@@ -1246,10 +1261,10 @@
         <v>0.0005697668442642861</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q8">
         <v>1.346998547516964E-14</v>
@@ -1258,10 +1273,10 @@
         <v>-2.616101958511456</v>
       </c>
       <c r="S8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U8">
         <v>1.826850878707894E-75</v>
@@ -1270,10 +1285,10 @@
         <v>0.152402554115701</v>
       </c>
       <c r="W8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Y8">
         <v>0.0006040271222392212</v>
@@ -1282,10 +1297,10 @@
         <v>-0.6078726742980095</v>
       </c>
       <c r="AA8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AB8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AC8">
         <v>0.02878762954655125</v>
@@ -1294,10 +1309,10 @@
         <v>0.07723276611382776</v>
       </c>
       <c r="AE8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AF8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AG8">
         <v>0.008348060303740305</v>
@@ -1306,7 +1321,7 @@
         <v>0.001293971855322156</v>
       </c>
       <c r="AI8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AK8">
         <v>0.1170666019777796</v>
@@ -1314,10 +1329,10 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>0.2147035199372997</v>
@@ -1332,10 +1347,10 @@
         <v>-0.04753953954204398</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I9">
         <v>8.799323447970588E-69</v>
@@ -1344,10 +1359,10 @@
         <v>0.005938457237606129</v>
       </c>
       <c r="K9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M9">
         <v>4.142572278114807E-12</v>
@@ -1356,10 +1371,10 @@
         <v>0.0003107306984592267</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q9">
         <v>4.036892201073927E-12</v>
@@ -1368,10 +1383,10 @@
         <v>0.7577771361092032</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U9">
         <v>8.547981923086256E-20</v>
@@ -1380,10 +1395,10 @@
         <v>0.05745287142026485</v>
       </c>
       <c r="W9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Y9">
         <v>0.03284352412458014</v>
@@ -1392,7 +1407,7 @@
         <v>-0.2560609739645046</v>
       </c>
       <c r="AA9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AC9">
         <v>0.12875029029489</v>
@@ -1401,10 +1416,10 @@
         <v>0.04415547991322162</v>
       </c>
       <c r="AE9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AF9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AG9">
         <v>0.01289566544940651</v>
@@ -1413,7 +1428,7 @@
         <v>-0.0007000815865924753</v>
       </c>
       <c r="AI9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AK9">
         <v>0.1620773637861845</v>
@@ -1421,10 +1436,10 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>0.6049553546031476</v>
@@ -1439,10 +1454,10 @@
         <v>-0.006071572838217493</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I10">
         <v>0.006359329001445982</v>
@@ -1451,10 +1466,10 @@
         <v>-0.01330893776524718</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M10">
         <v>1.776605897839431E-68</v>
@@ -1463,10 +1478,10 @@
         <v>0.0002590361458050593</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q10">
         <v>1.428234154658986E-11</v>
@@ -1475,10 +1490,10 @@
         <v>-3.373879094620659</v>
       </c>
       <c r="S10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="T10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U10">
         <v>1.976262583364986E-322</v>
@@ -1487,10 +1502,10 @@
         <v>0.09494968269543617</v>
       </c>
       <c r="W10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="X10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Y10">
         <v>3.928542927132261E-05</v>
@@ -1499,10 +1514,10 @@
         <v>-0.3518117003335053</v>
       </c>
       <c r="AA10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="AB10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AC10">
         <v>0.0148424474521775</v>
@@ -1511,10 +1526,10 @@
         <v>0.0330772862006062</v>
       </c>
       <c r="AE10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AF10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AG10">
         <v>0.02956140185377016</v>
@@ -1523,10 +1538,10 @@
         <v>0.001994053441914628</v>
       </c>
       <c r="AI10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AJ10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="AK10">
         <v>3.517625792160124E-06</v>
@@ -1534,10 +1549,10 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>0.1772021242589028</v>
@@ -1552,10 +1567,10 @@
         <v>-0.0424682563223264</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I11">
         <v>3.700699043234285E-56</v>
@@ -1564,10 +1579,10 @@
         <v>0.003810330728468005</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M11">
         <v>5.792769013199906E-06</v>
@@ -1576,10 +1591,10 @@
         <v>0.0003296310763475154</v>
       </c>
       <c r="O11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q11">
         <v>6.286199376622963E-13</v>
@@ -1588,10 +1603,10 @@
         <v>0.06768874976843403</v>
       </c>
       <c r="S11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="T11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="U11">
         <v>0.01395205599790157</v>
@@ -1600,10 +1615,10 @@
         <v>-0.3573401747519762</v>
       </c>
       <c r="W11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="X11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Y11">
         <v>0.03794741408251676</v>
@@ -1612,10 +1627,10 @@
         <v>0.05482291769034758</v>
       </c>
       <c r="AA11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AB11" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AC11">
         <v>0.00250910110558321</v>
@@ -1624,7 +1639,7 @@
         <v>-0.0007618797976859061</v>
       </c>
       <c r="AE11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AG11">
         <v>0.137026815798597</v>
@@ -1632,10 +1647,10 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>0.2147035199372997</v>
@@ -1650,10 +1665,10 @@
         <v>-0.04753953954204407</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I12">
         <v>8.799323447972345E-69</v>
@@ -1662,10 +1677,10 @@
         <v>0.005938457237606124</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M12">
         <v>4.142572278114777E-12</v>
@@ -1674,10 +1689,10 @@
         <v>0.0003107306984592273</v>
       </c>
       <c r="O12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q12">
         <v>4.036892201073707E-12</v>
@@ -1686,10 +1701,10 @@
         <v>0.05745287142026485</v>
       </c>
       <c r="S12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="T12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="U12">
         <v>0.0328435241245802</v>
@@ -1698,7 +1713,7 @@
         <v>-0.2560609739645043</v>
       </c>
       <c r="W12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="Y12">
         <v>0.1287502902948907</v>
@@ -1707,10 +1722,10 @@
         <v>0.04415547991322162</v>
       </c>
       <c r="AA12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AB12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AC12">
         <v>0.01289566544940665</v>
@@ -1719,7 +1734,7 @@
         <v>-0.0007000815865924622</v>
       </c>
       <c r="AE12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AG12">
         <v>0.1620773637861929</v>
@@ -1728,10 +1743,10 @@
         <v>0.7577771361092038</v>
       </c>
       <c r="AI12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AJ12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="AK12">
         <v>8.547981923086256E-20</v>
@@ -1752,24 +1767,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>-13.97698953761943</v>
@@ -1786,7 +1801,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>2.567281204183598</v>
@@ -1803,7 +1818,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>-0.1813356063920056</v>
@@ -1820,7 +1835,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0.01017486372989804</v>
@@ -1837,7 +1852,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>-13.30246450329206</v>
@@ -1854,7 +1869,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>1.924636689693848</v>
@@ -1871,7 +1886,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>-0.930796885552617</v>
@@ -1888,7 +1903,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>0.2974253892846115</v>
@@ -1905,7 +1920,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>-0.005395067678689072</v>
@@ -1935,24 +1950,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>2.650347470735377</v>
@@ -1969,7 +1984,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>-0.05361111238026152</v>
@@ -1986,7 +2001,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>-0.007370480527641051</v>
@@ -2003,7 +2018,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0.0005697668442642861</v>
@@ -2020,7 +2035,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>-2.616101958511456</v>
@@ -2037,7 +2052,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>0.152402554115701</v>
@@ -2054,7 +2069,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>-0.6078726742980095</v>
@@ -2071,7 +2086,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>0.07723276611382776</v>
@@ -2088,7 +2103,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>0.001293971855322156</v>
@@ -2118,24 +2133,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>2.822293117560656</v>
@@ -2152,7 +2167,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>-0.006071572838217493</v>
@@ -2169,7 +2184,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>-0.01330893776524718</v>
@@ -2186,7 +2201,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0.0002590361458050593</v>
@@ -2203,7 +2218,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>-3.373879094620659</v>
@@ -2220,7 +2235,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>0.09494968269543617</v>
@@ -2237,7 +2252,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>-0.3518117003335053</v>
@@ -2254,7 +2269,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>0.0330772862006062</v>
@@ -2271,7 +2286,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>0.001994053441914628</v>
@@ -2301,24 +2316,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>-0.1719456468252796</v>
@@ -2335,7 +2350,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>-0.04753953954204407</v>
@@ -2352,7 +2367,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>0.005938457237606124</v>
@@ -2369,7 +2384,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0.0003107306984592273</v>
@@ -2386,7 +2401,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>0.05745287142026485</v>
@@ -2403,7 +2418,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>-0.2560609739645043</v>
@@ -2420,7 +2435,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>0.04415547991322162</v>
@@ -2437,7 +2452,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <v>-0.0007000815865924622</v>
@@ -2454,7 +2469,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>0.7577771361092038</v>

</xml_diff>